<commit_message>
[feat] add detail site page
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -80,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +103,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -175,10 +183,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -193,8 +202,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,7 +511,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +669,7 @@
       <c r="S5" s="4"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -669,7 +680,10 @@
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="O1:S1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>